<commit_message>
[SSE] - fix: aggiunti run EnergiBridge registration (before) + script Python con media, varianza e deviazione standard
</commit_message>
<xml_diff>
--- a/Performance/energibridge/before/registration/registration_before_summary.xlsx
+++ b/Performance/energibridge/before/registration/registration_before_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antoniocaiazzo/Università/Ingegneria del Software/CineNow-Software-Dependability/Performance/energibridge/before/registration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB01E1B-FC83-7A46-B0A8-610AE737E461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{875A4F37-062D-064C-9ECF-9D3BA81FD0EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-3600" windowWidth="38400" windowHeight="21600" xr2:uid="{ED5DFBAC-3CB8-324A-9497-2D46862C50F5}"/>
   </bookViews>
@@ -657,7 +657,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="it-IT"/>
-              <a:t>Energia per run – guest navigation (before)</a:t>
+              <a:t>Energia per run – registration (before)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1230,7 +1230,7 @@
               <a:rPr lang="it-IT" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Energia vs durata - guest navigation (before)</a:t>
+              <a:t>Energia vs durata - registration (before)</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -1660,7 +1660,7 @@
               <a:rPr lang="it-IT" b="0" i="0" u="none" strike="noStrike">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Potenza media per run – guest navigation (before)</a:t>
+              <a:t>Potenza media per run – registration (before)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -4055,7 +4055,7 @@
   <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="164" workbookViewId="0">
-      <selection activeCell="O35" sqref="O35"/>
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>